<commit_message>
build: rewrite embedding build process + fetch latest Wikipedia articles
</commit_message>
<xml_diff>
--- a/knowledge/proprietary/_metadata.xlsx
+++ b/knowledge/proprietary/_metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/charnould/GitHub/pierre/knowledge/proprietary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AB0B0A0-985A-1848-B821-7904995230D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CD1E346-E8E6-744D-8531-A8A2305D2F63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2740" yWindow="1420" windowWidth="27500" windowHeight="17400" xr2:uid="{E5B0FB10-8797-D243-A0FA-6D923D5CC0EA}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
   <si>
     <t>test-markdown-file.md</t>
   </si>
@@ -50,9 +50,6 @@
     <t>test-word-file.docx</t>
   </si>
   <si>
-    <t>Ci-après les caractéristiques techniques d'un programme immobilier de Pierre Habitat :</t>
-  </si>
-  <si>
     <t>test-folder/test-excel-file-from-folder.xlsx</t>
   </si>
   <si>
@@ -62,9 +59,6 @@
     <t>public</t>
   </si>
   <si>
-    <t>Ci-après les noms des collaborateurs en charge chez Pierre Habitat :</t>
-  </si>
-  <si>
     <t>Chemin d'accès</t>
   </si>
   <si>
@@ -78,14 +72,6 @@
   </si>
   <si>
     <t>Ligne d'en-tête</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Applicable uniquement pour les fichiers XLS. Indiquer l'onglet.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Applicable uniquement pour les fichiers XLS. Indiquer la ligne d'en-tête.</t>
   </si>
   <si>
     <t xml:space="preserve">
@@ -93,20 +79,90 @@
   </si>
   <si>
     <t xml:space="preserve">
-Optionnelle et applicable principalement aux fichiers XLS. Afin d'aider l'IA à savoir le sujet couvert par le document.
-Indiquer en français et le plus clairement possible à quoi correspond un ligne du fichier.
-Ex : "Liste l'ensemble des élements techniques d'une résidence de Grand Dijon Habitat"</t>
+Doit correspondre précisément au chemin d'accès du fichier. Respecter les espaces et la casse.</t>
   </si>
   <si>
     <t xml:space="preserve">
-Doit correspondre précisément au chemin d'accès au fichier. Respecter les espaces et la casse.</t>
+Applicable uniquement aux fichiers XLS. Indiquer l'onglet concerné.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Applicable uniquement aux fichiers XLS. Indiquer quelle est la ligne de la ligne d'en-têtes.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">
+Optionnelle, applicable principalement aux fichiers XLS mais </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>extrêmement important</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">. Afin d'aider l'IA à comprendre le sujet couvert, indiquer le plus clairement possible à quoi correspond </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>une</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> ligne du fichier Excel.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+Ex : "Ci-après l'ensemble des élements et caractéristiques techniques d'une résidence de Pierre Habitat :"</t>
+    </r>
+  </si>
+  <si>
+    <t>Ci-après les caractéristiques techniques d'un programme immobilier de Pierre Habitat :</t>
+  </si>
+  <si>
+    <t>Ci-après les noms des collaborateurs en charge chez Pierre Habitat :</t>
+  </si>
+  <si>
+    <t>Ci-après la procédure et la répartition des responsabilités entre la société de télésurveillance et l'agent/cadre d'astreinte chez Pierre Habitat :</t>
+  </si>
+  <si>
+    <t>Ci-après les noms des agents et cadre d'astreinte pour la semaine considérée chez Pierre Habitat :</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -142,6 +198,21 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF0070C0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF0070C0"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -517,25 +588,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F3359B2-613C-1246-BB58-A3F329ACACAC}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="40.6640625" style="1" customWidth="1"/>
-    <col min="2" max="3" width="22.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="23.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="22.1640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="29.83203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="95.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="101.33203125" style="1" customWidth="1"/>
     <col min="6" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="5" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="5" customFormat="1" ht="78" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>13</v>
@@ -544,27 +616,27 @@
         <v>14</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>9</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -578,10 +650,10 @@
         <v>3</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -595,46 +667,84 @@
         <v>1</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="2">
+        <v>3</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2">
-        <v>3</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="2"/>
+      <c r="E5" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="6" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
+        <v>3</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2">
+        <v>5</v>
+      </c>
       <c r="D6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="2"/>
+        <v>4</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="7" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="2">
         <v>2</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
+      <c r="C7" s="2">
+        <v>5</v>
+      </c>
       <c r="D7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" s="2"/>
+        <v>4</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="2"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:E2" xr:uid="{0F3359B2-613C-1246-BB58-A3F329ACACAC}">
@@ -644,7 +754,7 @@
   </autoFilter>
   <dataConsolidate/>
   <dataValidations count="2">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C202" xr:uid="{49006576-7484-B84D-A51B-69FE1DA1041A}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C204" xr:uid="{49006576-7484-B84D-A51B-69FE1DA1041A}">
       <formula1>1</formula1>
       <formula2>10</formula2>
     </dataValidation>

</xml_diff>